<commit_message>
Update to soil c stats.
</commit_message>
<xml_diff>
--- a/07_calc_country_stats/02_soil_c_stats/02_combine_tile_stats/country_total_soil_c_hists_summary.xlsx
+++ b/07_calc_country_stats/02_soil_c_stats/02_combine_tile_stats/country_total_soil_c_hists_summary.xlsx
@@ -1170,10 +1170,10 @@
         <v>130</v>
       </c>
       <c r="D2">
-        <v>0.1191828382616863</v>
+        <v>0.04278358296573355</v>
       </c>
       <c r="E2">
-        <v>0.8435316415357005</v>
+        <v>0.9199308968316533</v>
       </c>
       <c r="F2">
         <v>0.03728552020261317</v>
@@ -1199,10 +1199,10 @@
         <v>131</v>
       </c>
       <c r="D3">
-        <v>0.6666666666666666</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="E3">
-        <v>0.3333333333333333</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1228,10 +1228,10 @@
         <v>132</v>
       </c>
       <c r="D4">
-        <v>0.2012078569334506</v>
+        <v>0.04526531808853709</v>
       </c>
       <c r="E4">
-        <v>0.7776722368806801</v>
+        <v>0.9336147757255937</v>
       </c>
       <c r="F4">
         <v>0.02111990618586925</v>
@@ -1257,10 +1257,10 @@
         <v>133</v>
       </c>
       <c r="D5">
-        <v>0.1152737752161383</v>
+        <v>0.0345821325648415</v>
       </c>
       <c r="E5">
-        <v>0.8847262247838616</v>
+        <v>0.9654178674351584</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1286,13 +1286,13 @@
         <v>134</v>
       </c>
       <c r="D6">
-        <v>0.4102508137394698</v>
+        <v>5.758948830587851E-07</v>
       </c>
       <c r="E6">
-        <v>0.06697254363555528</v>
+        <v>0.06743383543688537</v>
       </c>
       <c r="F6">
-        <v>0.5212597355029981</v>
+        <v>0.9310486815462548</v>
       </c>
       <c r="G6">
         <v>0.00151690712197684</v>
@@ -1315,10 +1315,10 @@
         <v>135</v>
       </c>
       <c r="D7">
-        <v>0.2214292868589744</v>
+        <v>0.03902493990384615</v>
       </c>
       <c r="E7">
-        <v>0.7160581931089743</v>
+        <v>0.8984625400641025</v>
       </c>
       <c r="F7">
         <v>0.06191155849358974</v>
@@ -1344,10 +1344,10 @@
         <v>136</v>
       </c>
       <c r="D8">
-        <v>0.2097096371021738</v>
+        <v>0.001722239581008496</v>
       </c>
       <c r="E8">
-        <v>0.6541013852311446</v>
+        <v>0.8620887827523099</v>
       </c>
       <c r="F8">
         <v>0.1361889776666815</v>
@@ -1373,10 +1373,10 @@
         <v>137</v>
       </c>
       <c r="D9">
-        <v>0.1256447426671644</v>
+        <v>0.01462660914401785</v>
       </c>
       <c r="E9">
-        <v>0.8235275735453685</v>
+        <v>0.934545707068515</v>
       </c>
       <c r="F9">
         <v>0.05082768378746712</v>
@@ -1402,10 +1402,10 @@
         <v>138</v>
       </c>
       <c r="D10">
-        <v>0.04155720085980415</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0.6995132717854113</v>
+        <v>0.7410704726452155</v>
       </c>
       <c r="F10">
         <v>0.2589295273547845</v>
@@ -1431,10 +1431,10 @@
         <v>139</v>
       </c>
       <c r="D11">
-        <v>0.2642851023729975</v>
+        <v>0.1579012951410793</v>
       </c>
       <c r="E11">
-        <v>0.7254970678255181</v>
+        <v>0.8318808750574364</v>
       </c>
       <c r="F11">
         <v>0.01021782980148439</v>
@@ -1460,10 +1460,10 @@
         <v>140</v>
       </c>
       <c r="D12">
-        <v>0.4894298526585522</v>
+        <v>0.0877642536835362</v>
       </c>
       <c r="E12">
-        <v>0.5105701473414478</v>
+        <v>0.9122357463164638</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1489,10 +1489,10 @@
         <v>141</v>
       </c>
       <c r="D13">
-        <v>0.6737864250731955</v>
+        <v>0.4242766233361111</v>
       </c>
       <c r="E13">
-        <v>0.3262091185789598</v>
+        <v>0.5757189203160442</v>
       </c>
       <c r="F13">
         <v>4.456347844687365E-06</v>
@@ -1518,10 +1518,10 @@
         <v>142</v>
       </c>
       <c r="D14">
-        <v>0.7996286083104251</v>
+        <v>0.3723480446184658</v>
       </c>
       <c r="E14">
-        <v>0.2001569623076032</v>
+        <v>0.6274375259995626</v>
       </c>
       <c r="F14">
         <v>0.0002144293819716353</v>
@@ -1547,10 +1547,10 @@
         <v>143</v>
       </c>
       <c r="D15">
-        <v>0.3612880458756065</v>
+        <v>0.2208381120423467</v>
       </c>
       <c r="E15">
-        <v>0.6384649316277018</v>
+        <v>0.7789148654609617</v>
       </c>
       <c r="F15">
         <v>0.000247022496691663</v>
@@ -1576,10 +1576,10 @@
         <v>144</v>
       </c>
       <c r="D16">
-        <v>0.1382532891655116</v>
+        <v>0.002424265717971323</v>
       </c>
       <c r="E16">
-        <v>0.8334674542567579</v>
+        <v>0.9692964777042982</v>
       </c>
       <c r="F16">
         <v>0.02827925657773048</v>
@@ -1605,10 +1605,10 @@
         <v>145</v>
       </c>
       <c r="D17">
-        <v>0.04577098567415171</v>
+        <v>0.000239096216302377</v>
       </c>
       <c r="E17">
-        <v>0.9191854788897965</v>
+        <v>0.9647173683476459</v>
       </c>
       <c r="F17">
         <v>0.03504353543605172</v>
@@ -1634,10 +1634,10 @@
         <v>146</v>
       </c>
       <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1663,10 +1663,10 @@
         <v>147</v>
       </c>
       <c r="D19">
-        <v>0.1781881517865602</v>
+        <v>0.1139040511882465</v>
       </c>
       <c r="E19">
-        <v>0.8215290885373017</v>
+        <v>0.8858131891356154</v>
       </c>
       <c r="F19">
         <v>0.0002827596761381441</v>
@@ -1692,13 +1692,13 @@
         <v>148</v>
       </c>
       <c r="D20">
-        <v>0.3651807556401196</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>0.3632780646914923</v>
       </c>
       <c r="F20">
-        <v>0.2715411796683881</v>
+        <v>0.6367219353085077</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1721,10 +1721,10 @@
         <v>149</v>
       </c>
       <c r="D21">
-        <v>0.1513984882850131</v>
+        <v>0.0003092063049489095</v>
       </c>
       <c r="E21">
-        <v>0.4945334827532588</v>
+        <v>0.6456227647333229</v>
       </c>
       <c r="F21">
         <v>0.3540644543223646</v>
@@ -1750,10 +1750,10 @@
         <v>150</v>
       </c>
       <c r="D22">
-        <v>0.1278765502903434</v>
+        <v>0.02771405357612254</v>
       </c>
       <c r="E22">
-        <v>0.6388630009319665</v>
+        <v>0.7390254976461873</v>
       </c>
       <c r="F22">
         <v>0.2332604487776901</v>
@@ -1779,13 +1779,13 @@
         <v>151</v>
       </c>
       <c r="D23">
-        <v>0.1562514293743851</v>
+        <v>0.005003908140146124</v>
       </c>
       <c r="E23">
-        <v>0.4900424454611134</v>
+        <v>0.6074997113092249</v>
       </c>
       <c r="F23">
-        <v>0.3530183604068201</v>
+        <v>0.3868086157929476</v>
       </c>
       <c r="G23">
         <v>0.0006877647576814355</v>
@@ -1808,10 +1808,10 @@
         <v>152</v>
       </c>
       <c r="D24">
-        <v>0.8225665427071264</v>
+        <v>0.7835944934113391</v>
       </c>
       <c r="E24">
-        <v>0.1694366387028702</v>
+        <v>0.2084086879986574</v>
       </c>
       <c r="F24">
         <v>0.007996818590003374</v>
@@ -1837,10 +1837,10 @@
         <v>153</v>
       </c>
       <c r="D25">
-        <v>0.1339185672880147</v>
+        <v>0.01910344380550231</v>
       </c>
       <c r="E25">
-        <v>0.7534701965904567</v>
+        <v>0.868285320072969</v>
       </c>
       <c r="F25">
         <v>0.1126112361215287</v>
@@ -1866,10 +1866,10 @@
         <v>154</v>
       </c>
       <c r="D26">
-        <v>0.385488481587355</v>
+        <v>0.0878594249201278</v>
       </c>
       <c r="E26">
-        <v>0.6144274424079368</v>
+        <v>0.912056499075164</v>
       </c>
       <c r="F26">
         <v>8.407600470825626E-05</v>
@@ -1895,10 +1895,10 @@
         <v>155</v>
       </c>
       <c r="D27">
-        <v>0.13360127042758</v>
+        <v>0.05310821020819342</v>
       </c>
       <c r="E27">
-        <v>0.810140684463846</v>
+        <v>0.8906337446832326</v>
       </c>
       <c r="F27">
         <v>0.05625804510857399</v>
@@ -1924,10 +1924,10 @@
         <v>156</v>
       </c>
       <c r="D28">
-        <v>0.1161330062807299</v>
+        <v>0.01223147404661599</v>
       </c>
       <c r="E28">
-        <v>0.7370453070517968</v>
+        <v>0.8409468392859107</v>
       </c>
       <c r="F28">
         <v>0.1468216866674733</v>
@@ -1953,10 +1953,10 @@
         <v>157</v>
       </c>
       <c r="D29">
-        <v>0.08909194745859508</v>
+        <v>0.006282124500285551</v>
       </c>
       <c r="E29">
-        <v>0.9086236436322102</v>
+        <v>0.9914334665905197</v>
       </c>
       <c r="F29">
         <v>0.002284408909194746</v>
@@ -1982,10 +1982,10 @@
         <v>158</v>
       </c>
       <c r="D30">
-        <v>0.5939937810266761</v>
+        <v>0.1539468659647591</v>
       </c>
       <c r="E30">
-        <v>0.4060062189733239</v>
+        <v>0.8460531340352409</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2011,10 +2011,10 @@
         <v>159</v>
       </c>
       <c r="D31">
-        <v>0.4618629857431321</v>
+        <v>0.4361607031472481</v>
       </c>
       <c r="E31">
-        <v>0.5377163028674622</v>
+        <v>0.5634185854633461</v>
       </c>
       <c r="F31">
         <v>0.0004207113894058161</v>
@@ -2040,10 +2040,10 @@
         <v>160</v>
       </c>
       <c r="D32">
-        <v>0.2629312384648148</v>
+        <v>0.001703658132601391</v>
       </c>
       <c r="E32">
-        <v>0.5480573564904643</v>
+        <v>0.8092849368226775</v>
       </c>
       <c r="F32">
         <v>0.189011405044721</v>
@@ -2069,10 +2069,10 @@
         <v>161</v>
       </c>
       <c r="D33">
-        <v>0.7455001139211666</v>
+        <v>0.002961950330371383</v>
       </c>
       <c r="E33">
-        <v>0.2540442014126225</v>
+        <v>0.9965823650034177</v>
       </c>
       <c r="F33">
         <v>0.000455684666210982</v>
@@ -2098,13 +2098,13 @@
         <v>162</v>
       </c>
       <c r="D34">
-        <v>0.07417352342631317</v>
+        <v>0.001311031896641247</v>
       </c>
       <c r="E34">
-        <v>0.6466477255118942</v>
+        <v>0.6950578592048884</v>
       </c>
       <c r="F34">
-        <v>0.2791368864822897</v>
+        <v>0.3035892443189675</v>
       </c>
       <c r="G34">
         <v>4.186457950292064E-05</v>
@@ -2127,10 +2127,10 @@
         <v>163</v>
       </c>
       <c r="D35">
-        <v>0.2597064069145287</v>
+        <v>0.01234737275346412</v>
       </c>
       <c r="E35">
-        <v>0.7391960488407189</v>
+        <v>0.9865550830017835</v>
       </c>
       <c r="F35">
         <v>0.001097544244752367</v>
@@ -2156,10 +2156,10 @@
         <v>164</v>
       </c>
       <c r="D36">
-        <v>0.2370305862395469</v>
+        <v>0.0004155264122006223</v>
       </c>
       <c r="E36">
-        <v>0.6980800875571095</v>
+        <v>0.9346951473844557</v>
       </c>
       <c r="F36">
         <v>0.06488932620334363</v>
@@ -2185,10 +2185,10 @@
         <v>165</v>
       </c>
       <c r="D37">
-        <v>0.1349195370498455</v>
+        <v>0.0441153561917153</v>
       </c>
       <c r="E37">
-        <v>0.8249941738667703</v>
+        <v>0.9157983547249006</v>
       </c>
       <c r="F37">
         <v>0.04008628908338412</v>
@@ -2214,10 +2214,10 @@
         <v>166</v>
       </c>
       <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
         <v>1</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2243,10 +2243,10 @@
         <v>167</v>
       </c>
       <c r="D39">
-        <v>0.3656845591743935</v>
+        <v>0.2446341189569513</v>
       </c>
       <c r="E39">
-        <v>0.6279180194425472</v>
+        <v>0.7489684596599894</v>
       </c>
       <c r="F39">
         <v>0.006392743195576306</v>
@@ -2272,10 +2272,10 @@
         <v>168</v>
       </c>
       <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
         <v>1</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2301,10 +2301,10 @@
         <v>169</v>
       </c>
       <c r="D41">
-        <v>0.1811539902585238</v>
+        <v>0.03784188834769577</v>
       </c>
       <c r="E41">
-        <v>0.8062944923192207</v>
+        <v>0.9496065942300487</v>
       </c>
       <c r="F41">
         <v>0.01255151742225553</v>
@@ -2330,10 +2330,10 @@
         <v>170</v>
       </c>
       <c r="D42">
-        <v>0.4504138449962378</v>
+        <v>0.1385001254075746</v>
       </c>
       <c r="E42">
-        <v>0.5416729370453975</v>
+        <v>0.8535866566340607</v>
       </c>
       <c r="F42">
         <v>0.007913217958364685</v>
@@ -2359,10 +2359,10 @@
         <v>171</v>
       </c>
       <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>1</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2388,10 +2388,10 @@
         <v>172</v>
       </c>
       <c r="D44">
-        <v>0.4914317302377004</v>
+        <v>0.1840796019900497</v>
       </c>
       <c r="E44">
-        <v>0.5085682697622996</v>
+        <v>0.8159203980099502</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2417,10 +2417,10 @@
         <v>173</v>
       </c>
       <c r="D45">
-        <v>0.3180405007262861</v>
+        <v>0.2101998657055938</v>
       </c>
       <c r="E45">
-        <v>0.6785807273823553</v>
+        <v>0.7864213624030476</v>
       </c>
       <c r="F45">
         <v>0.003378771891358566</v>
@@ -2446,13 +2446,13 @@
         <v>174</v>
       </c>
       <c r="D46">
-        <v>0.2522171038025185</v>
+        <v>0.0007192315602081235</v>
       </c>
       <c r="E46">
-        <v>0.306977996497558</v>
+        <v>0.3077336730902896</v>
       </c>
       <c r="F46">
-        <v>0.4407639920103563</v>
+        <v>0.6915061876599351</v>
       </c>
       <c r="G46">
         <v>4.090768956716318E-05</v>
@@ -2475,10 +2475,10 @@
         <v>175</v>
       </c>
       <c r="D47">
-        <v>0.2157434402332362</v>
+        <v>0.02623906705539359</v>
       </c>
       <c r="E47">
-        <v>0.7842565597667639</v>
+        <v>0.9737609329446064</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2504,10 +2504,10 @@
         <v>176</v>
       </c>
       <c r="D48">
-        <v>0.1372412445268011</v>
+        <v>0.0259584596210513</v>
       </c>
       <c r="E48">
-        <v>0.8602819149846217</v>
+        <v>0.9715646998903715</v>
       </c>
       <c r="F48">
         <v>0.002476840488577185</v>
@@ -2533,10 +2533,10 @@
         <v>177</v>
       </c>
       <c r="D49">
-        <v>0.4231306334899073</v>
+        <v>0.1679573441665609</v>
       </c>
       <c r="E49">
-        <v>0.5768693665100927</v>
+        <v>0.8320426558334392</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2562,10 +2562,10 @@
         <v>178</v>
       </c>
       <c r="D50">
-        <v>0.4303797468354431</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0.3649789029535865</v>
+        <v>0.7953586497890295</v>
       </c>
       <c r="F50">
         <v>0.2046413502109705</v>
@@ -2591,10 +2591,10 @@
         <v>179</v>
       </c>
       <c r="D51">
-        <v>0.1120435709452412</v>
+        <v>0.03732072265495821</v>
       </c>
       <c r="E51">
-        <v>0.8875163441921518</v>
+        <v>0.9622391924824347</v>
       </c>
       <c r="F51">
         <v>0.0004400848626070322</v>
@@ -2620,10 +2620,10 @@
         <v>180</v>
       </c>
       <c r="D52">
-        <v>0.1259114176557977</v>
+        <v>0.006488341167715426</v>
       </c>
       <c r="E52">
-        <v>0.6049342658355008</v>
+        <v>0.7243573423235832</v>
       </c>
       <c r="F52">
         <v>0.2691477819227717</v>
@@ -2649,10 +2649,10 @@
         <v>181</v>
       </c>
       <c r="D53">
-        <v>0.927536231884058</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>0.07246376811594203</v>
+        <v>1</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2678,10 +2678,10 @@
         <v>182</v>
       </c>
       <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
         <v>1</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2707,10 +2707,10 @@
         <v>183</v>
       </c>
       <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
         <v>1</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2736,10 +2736,10 @@
         <v>184</v>
       </c>
       <c r="D56">
-        <v>0.05980812398142739</v>
+        <v>0.00488607361397251</v>
       </c>
       <c r="E56">
-        <v>0.8940241689984932</v>
+        <v>0.9489462193659481</v>
       </c>
       <c r="F56">
         <v>0.04616770702007934</v>
@@ -2765,10 +2765,10 @@
         <v>185</v>
       </c>
       <c r="D57">
-        <v>0.200793982448809</v>
+        <v>0.004701211867948182</v>
       </c>
       <c r="E57">
-        <v>0.6784371082323444</v>
+        <v>0.8745298788132052</v>
       </c>
       <c r="F57">
         <v>0.1207689093188466</v>
@@ -2794,10 +2794,10 @@
         <v>186</v>
       </c>
       <c r="D58">
-        <v>0.3192281668863904</v>
+        <v>0.2181922178035908</v>
       </c>
       <c r="E58">
-        <v>0.6297564341544958</v>
+        <v>0.7307923832372953</v>
       </c>
       <c r="F58">
         <v>0.05101150363040106</v>
@@ -2823,10 +2823,10 @@
         <v>187</v>
       </c>
       <c r="D59">
-        <v>0.9604790024082077</v>
+        <v>0.001220598423118794</v>
       </c>
       <c r="E59">
-        <v>0.0395209975917923</v>
+        <v>0.9987794015768812</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>188</v>
       </c>
       <c r="D60">
-        <v>0.1570707070707071</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>0.04191919191919192</v>
+        <v>0.198989898989899</v>
       </c>
       <c r="F60">
         <v>0.8005050505050505</v>
@@ -2910,10 +2910,10 @@
         <v>190</v>
       </c>
       <c r="D62">
-        <v>0.7526561835954101</v>
+        <v>0.4351891202719932</v>
       </c>
       <c r="E62">
-        <v>0.2473438164045899</v>
+        <v>0.5648108797280068</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2939,13 +2939,13 @@
         <v>191</v>
       </c>
       <c r="D63">
-        <v>0.8975214128704616</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>0.04730863769748027</v>
+        <v>0.921462680425767</v>
       </c>
       <c r="F63">
-        <v>0.05516994943205813</v>
+        <v>0.07853731957423309</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2968,10 +2968,10 @@
         <v>192</v>
       </c>
       <c r="D64">
-        <v>0.05334714580917422</v>
+        <v>7.520206467813516E-05</v>
       </c>
       <c r="E64">
-        <v>0.8225122285096477</v>
+        <v>0.8757841722541437</v>
       </c>
       <c r="F64">
         <v>0.1241406256811781</v>
@@ -2997,10 +2997,10 @@
         <v>193</v>
       </c>
       <c r="D65">
-        <v>0.4759655991203234</v>
+        <v>0.3968159531689074</v>
       </c>
       <c r="E65">
-        <v>0.5240344008796766</v>
+        <v>0.6031840468310925</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -3026,10 +3026,10 @@
         <v>194</v>
       </c>
       <c r="D66">
-        <v>0.7759760379146919</v>
+        <v>0.7740514881516588</v>
       </c>
       <c r="E66">
-        <v>0.2238862559241706</v>
+        <v>0.2258108056872038</v>
       </c>
       <c r="F66">
         <v>0.0001377061611374408</v>
@@ -3055,13 +3055,13 @@
         <v>195</v>
       </c>
       <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
         <v>1</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3084,10 +3084,10 @@
         <v>196</v>
       </c>
       <c r="D68">
-        <v>0.260815074288808</v>
+        <v>0.1490121090864533</v>
       </c>
       <c r="E68">
-        <v>0.733225053193363</v>
+        <v>0.8450280183957176</v>
       </c>
       <c r="F68">
         <v>0.005959789835987338</v>
@@ -3113,10 +3113,10 @@
         <v>197</v>
       </c>
       <c r="D69">
-        <v>0.2478632478632479</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="E69">
-        <v>0.7521367521367521</v>
+        <v>0.9743589743589743</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3142,10 +3142,10 @@
         <v>198</v>
       </c>
       <c r="D70">
-        <v>0.1595845325658245</v>
+        <v>0.06823965995096472</v>
       </c>
       <c r="E70">
-        <v>0.8376638951071315</v>
+        <v>0.9290087677219913</v>
       </c>
       <c r="F70">
         <v>0.002751572327044025</v>
@@ -3171,10 +3171,10 @@
         <v>199</v>
       </c>
       <c r="D71">
-        <v>0.8227582590456214</v>
+        <v>0.04745673833245936</v>
       </c>
       <c r="E71">
-        <v>0.1772417409543786</v>
+        <v>0.9525432616675407</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -3200,10 +3200,10 @@
         <v>200</v>
       </c>
       <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
         <v>1</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3229,10 +3229,10 @@
         <v>201</v>
       </c>
       <c r="D73">
-        <v>0.2235909157966313</v>
+        <v>0.0001892401060151562</v>
       </c>
       <c r="E73">
-        <v>0.5785900933821921</v>
+        <v>0.8019917690728082</v>
       </c>
       <c r="F73">
         <v>0.1978189908211766</v>
@@ -3258,10 +3258,10 @@
         <v>202</v>
       </c>
       <c r="D74">
-        <v>0.1392405063291139</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>0.8500486854917235</v>
+        <v>0.9892891918208374</v>
       </c>
       <c r="F74">
         <v>0.01071080817916261</v>
@@ -3287,10 +3287,10 @@
         <v>203</v>
       </c>
       <c r="D75">
-        <v>0.1092097012359164</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>0.03796751421000465</v>
+        <v>0.1471772154459211</v>
       </c>
       <c r="F75">
         <v>0.8528227845540789</v>
@@ -3316,10 +3316,10 @@
         <v>204</v>
       </c>
       <c r="D76">
-        <v>0.5102413568166992</v>
+        <v>0.1140247879973907</v>
       </c>
       <c r="E76">
-        <v>0.4897586431833007</v>
+        <v>0.8859752120026093</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3345,10 +3345,10 @@
         <v>205</v>
       </c>
       <c r="D77">
-        <v>0.2142857142857143</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>0.7857142857142857</v>
+        <v>1</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3374,10 +3374,10 @@
         <v>206</v>
       </c>
       <c r="D78">
-        <v>0.1175949026802432</v>
+        <v>0.03288639032603415</v>
       </c>
       <c r="E78">
-        <v>0.7108799102026572</v>
+        <v>0.7955884225568661</v>
       </c>
       <c r="F78">
         <v>0.1715251871170997</v>
@@ -3403,10 +3403,10 @@
         <v>207</v>
       </c>
       <c r="D79">
-        <v>0.2026392069226414</v>
+        <v>0.0276566187486534</v>
       </c>
       <c r="E79">
-        <v>0.7607621369195849</v>
+        <v>0.9357447250935729</v>
       </c>
       <c r="F79">
         <v>0.03656170300184891</v>
@@ -3432,10 +3432,10 @@
         <v>208</v>
       </c>
       <c r="D80">
-        <v>0.5771810016390271</v>
+        <v>0.5176501896820321</v>
       </c>
       <c r="E80">
-        <v>0.4228151538878516</v>
+        <v>0.4823459658448465</v>
       </c>
       <c r="F80">
         <v>3.844473121366172E-06</v>
@@ -3461,10 +3461,10 @@
         <v>209</v>
       </c>
       <c r="D81">
-        <v>0.1244994928193903</v>
+        <v>5.338743259836634E-05</v>
       </c>
       <c r="E81">
-        <v>0.4031551972665635</v>
+        <v>0.5276013026533554</v>
       </c>
       <c r="F81">
         <v>0.4723453099140462</v>
@@ -3490,10 +3490,10 @@
         <v>210</v>
       </c>
       <c r="D82">
-        <v>0.7076744965882865</v>
+        <v>0.641458274220738</v>
       </c>
       <c r="E82">
-        <v>0.2923163994398023</v>
+        <v>0.3585326218073508</v>
       </c>
       <c r="F82">
         <v>9.103971911211997E-06</v>
@@ -3519,10 +3519,10 @@
         <v>211</v>
       </c>
       <c r="D83">
-        <v>0.3074949078254595</v>
+        <v>0.2234490415150216</v>
       </c>
       <c r="E83">
-        <v>0.6807156938573174</v>
+        <v>0.7647615601677553</v>
       </c>
       <c r="F83">
         <v>0.01178939831722306</v>
@@ -3548,10 +3548,10 @@
         <v>212</v>
       </c>
       <c r="D84">
-        <v>0.05708289221968389</v>
+        <v>0.001062387399936851</v>
       </c>
       <c r="E84">
-        <v>0.8881038613695882</v>
+        <v>0.9441243661893353</v>
       </c>
       <c r="F84">
         <v>0.05481324641072789</v>
@@ -3577,10 +3577,10 @@
         <v>213</v>
       </c>
       <c r="D85">
-        <v>0.172147001934236</v>
+        <v>0.007736943907156673</v>
       </c>
       <c r="E85">
-        <v>0.8147969052224371</v>
+        <v>0.9792069632495164</v>
       </c>
       <c r="F85">
         <v>0.01305609284332689</v>
@@ -3606,10 +3606,10 @@
         <v>214</v>
       </c>
       <c r="D86">
-        <v>0.4611107205883985</v>
+        <v>0.3790812192694594</v>
       </c>
       <c r="E86">
-        <v>0.5376276855116485</v>
+        <v>0.6196571868305876</v>
       </c>
       <c r="F86">
         <v>0.001261593899953014</v>
@@ -3635,10 +3635,10 @@
         <v>215</v>
       </c>
       <c r="D87">
-        <v>0.7966018159781059</v>
+        <v>0.4767136097106288</v>
       </c>
       <c r="E87">
-        <v>0.2032537515224972</v>
+        <v>0.5231419577899743</v>
       </c>
       <c r="F87">
         <v>0.0001444324993969571</v>
@@ -3664,10 +3664,10 @@
         <v>216</v>
       </c>
       <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
         <v>1</v>
-      </c>
-      <c r="E88">
-        <v>0</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3693,10 +3693,10 @@
         <v>217</v>
       </c>
       <c r="D89">
-        <v>0.3538048076444533</v>
+        <v>0.02145855107085386</v>
       </c>
       <c r="E89">
-        <v>0.6418321471822691</v>
+        <v>0.9741784037558685</v>
       </c>
       <c r="F89">
         <v>0.004363045173277592</v>
@@ -3722,10 +3722,10 @@
         <v>218</v>
       </c>
       <c r="D90">
-        <v>0.5994865211810013</v>
+        <v>0.03953786906290115</v>
       </c>
       <c r="E90">
-        <v>0.4001283697047497</v>
+        <v>0.9600770218228498</v>
       </c>
       <c r="F90">
         <v>0.0003851091142490372</v>
@@ -3751,10 +3751,10 @@
         <v>219</v>
       </c>
       <c r="D91">
-        <v>0.6689209014653703</v>
+        <v>0.4642338945897356</v>
       </c>
       <c r="E91">
-        <v>0.3304700820659774</v>
+        <v>0.5351570889416121</v>
       </c>
       <c r="F91">
         <v>0.0006090164686522889</v>
@@ -3780,10 +3780,10 @@
         <v>220</v>
       </c>
       <c r="D92">
-        <v>0.06077315997213838</v>
+        <v>5.804504295333179E-05</v>
       </c>
       <c r="E92">
-        <v>0.9031808683538426</v>
+        <v>0.9638959832830276</v>
       </c>
       <c r="F92">
         <v>0.03604597167401904</v>
@@ -3809,10 +3809,10 @@
         <v>221</v>
       </c>
       <c r="D93">
-        <v>0.1613082704455681</v>
+        <v>0.06808785331140586</v>
       </c>
       <c r="E93">
-        <v>0.7768301492399674</v>
+        <v>0.8700505663741297</v>
       </c>
       <c r="F93">
         <v>0.06186158031446444</v>
@@ -3838,10 +3838,10 @@
         <v>222</v>
       </c>
       <c r="D94">
-        <v>0.4103125194934814</v>
+        <v>0.1800617553490113</v>
       </c>
       <c r="E94">
-        <v>0.5895614746428794</v>
+        <v>0.8198122387873495</v>
       </c>
       <c r="F94">
         <v>0.0001260058636391991</v>
@@ -3867,10 +3867,10 @@
         <v>223</v>
       </c>
       <c r="D95">
-        <v>0.3113808197373657</v>
+        <v>0.2736147035415837</v>
       </c>
       <c r="E95">
-        <v>0.6884052924791086</v>
+        <v>0.7261714086748906</v>
       </c>
       <c r="F95">
         <v>0.0002138877835256665</v>
@@ -3896,10 +3896,10 @@
         <v>224</v>
       </c>
       <c r="D96">
-        <v>0.2756750579214761</v>
+        <v>0.189296734579381</v>
       </c>
       <c r="E96">
-        <v>0.7242210470540565</v>
+        <v>0.8105993703961517</v>
       </c>
       <c r="F96">
         <v>0.0001038950244672783</v>
@@ -3925,10 +3925,10 @@
         <v>225</v>
       </c>
       <c r="D97">
-        <v>0.2717344498228247</v>
+        <v>0.04193580185424416</v>
       </c>
       <c r="E97">
-        <v>0.7115078315096992</v>
+        <v>0.9413064794782798</v>
       </c>
       <c r="F97">
         <v>0.01675771866747602</v>
@@ -3954,10 +3954,10 @@
         <v>226</v>
       </c>
       <c r="D98">
-        <v>0.3099613755763242</v>
+        <v>0.2077290912068217</v>
       </c>
       <c r="E98">
-        <v>0.6897231390494275</v>
+        <v>0.79195542341893</v>
       </c>
       <c r="F98">
         <v>0.000315485374248281</v>
@@ -3983,10 +3983,10 @@
         <v>227</v>
       </c>
       <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
         <v>1</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -4012,10 +4012,10 @@
         <v>228</v>
       </c>
       <c r="D100">
-        <v>0.4574468085106383</v>
+        <v>0.01861702127659574</v>
       </c>
       <c r="E100">
-        <v>0.5425531914893617</v>
+        <v>0.9813829787234043</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -4041,10 +4041,10 @@
         <v>229</v>
       </c>
       <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
         <v>1</v>
-      </c>
-      <c r="E101">
-        <v>0</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -4070,10 +4070,10 @@
         <v>230</v>
       </c>
       <c r="D102">
-        <v>0.5713594846989422</v>
+        <v>0.541077680259343</v>
       </c>
       <c r="E102">
-        <v>0.4274663714558756</v>
+        <v>0.4577481758954747</v>
       </c>
       <c r="F102">
         <v>0.001174143845182258</v>
@@ -4099,10 +4099,10 @@
         <v>231</v>
       </c>
       <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
         <v>1</v>
-      </c>
-      <c r="E103">
-        <v>0</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -4128,10 +4128,10 @@
         <v>232</v>
       </c>
       <c r="D104">
-        <v>0.2934944296881522</v>
+        <v>0.2373446833718658</v>
       </c>
       <c r="E104">
-        <v>0.6504324786326322</v>
+        <v>0.7065822249489186</v>
       </c>
       <c r="F104">
         <v>0.05607048560128464</v>
@@ -4157,10 +4157,10 @@
         <v>233</v>
       </c>
       <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
         <v>1</v>
-      </c>
-      <c r="E105">
-        <v>0</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -4186,10 +4186,10 @@
         <v>234</v>
       </c>
       <c r="D106">
-        <v>0.2404212300362243</v>
+        <v>0.05287634714909201</v>
       </c>
       <c r="E106">
-        <v>0.7506830148580574</v>
+        <v>0.9382278977451898</v>
       </c>
       <c r="F106">
         <v>0.008895755105718245</v>
@@ -4215,10 +4215,10 @@
         <v>235</v>
       </c>
       <c r="D107">
-        <v>0.3165638597165674</v>
+        <v>0.004543309976060251</v>
       </c>
       <c r="E107">
-        <v>0.6833662432068779</v>
+        <v>0.995386792947385</v>
       </c>
       <c r="F107">
         <v>6.98970765547731E-05</v>
@@ -4244,10 +4244,10 @@
         <v>236</v>
       </c>
       <c r="D108">
-        <v>0.162578956221598</v>
+        <v>0.01294391972524758</v>
       </c>
       <c r="E108">
-        <v>0.6468055925309302</v>
+        <v>0.7964406290272805</v>
       </c>
       <c r="F108">
         <v>0.1906154512474719</v>
@@ -4273,13 +4273,13 @@
         <v>237</v>
       </c>
       <c r="D109">
-        <v>0.05260195974576271</v>
+        <v>0</v>
       </c>
       <c r="E109">
         <v>0.1182799258474576</v>
       </c>
       <c r="F109">
-        <v>0.7856362552966102</v>
+        <v>0.8382382150423728</v>
       </c>
       <c r="G109">
         <v>0.04348185911016949</v>
@@ -4302,13 +4302,13 @@
         <v>238</v>
       </c>
       <c r="D110">
-        <v>0.1080366893109617</v>
+        <v>0.01038606362322498</v>
       </c>
       <c r="E110">
-        <v>0.7712483630535791</v>
+        <v>0.8601905277245959</v>
       </c>
       <c r="F110">
-        <v>0.1206128635545009</v>
+        <v>0.1293213245712208</v>
       </c>
       <c r="G110">
         <v>0.0001020840809583127</v>
@@ -4331,10 +4331,10 @@
         <v>239</v>
       </c>
       <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
         <v>1</v>
-      </c>
-      <c r="E111">
-        <v>0</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -4360,10 +4360,10 @@
         <v>240</v>
       </c>
       <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
         <v>1</v>
-      </c>
-      <c r="E112">
-        <v>0</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -4389,13 +4389,13 @@
         <v>241</v>
       </c>
       <c r="D113">
-        <v>0.3512226011281974</v>
+        <v>0</v>
       </c>
       <c r="E113">
         <v>0.04777120017660762</v>
       </c>
       <c r="F113">
-        <v>0.6002509687276699</v>
+        <v>0.9514735698558673</v>
       </c>
       <c r="G113">
         <v>0.0007552299675251114</v>
@@ -4418,10 +4418,10 @@
         <v>242</v>
       </c>
       <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
         <v>1</v>
-      </c>
-      <c r="E114">
-        <v>0</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -4447,10 +4447,10 @@
         <v>243</v>
       </c>
       <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
         <v>1</v>
-      </c>
-      <c r="E115">
-        <v>0</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -4476,10 +4476,10 @@
         <v>244</v>
       </c>
       <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
         <v>1</v>
-      </c>
-      <c r="E116">
-        <v>0</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -4505,10 +4505,10 @@
         <v>245</v>
       </c>
       <c r="D117">
-        <v>0.3327876146430233</v>
+        <v>0.1963599378367162</v>
       </c>
       <c r="E117">
-        <v>0.6664441381767208</v>
+        <v>0.8028718149830278</v>
       </c>
       <c r="F117">
         <v>0.0007682471802559352</v>
@@ -4534,10 +4534,10 @@
         <v>246</v>
       </c>
       <c r="D118">
-        <v>0.2297357814599194</v>
+        <v>0.0625167935512763</v>
       </c>
       <c r="E118">
-        <v>0.7683833407971339</v>
+        <v>0.935602328705777</v>
       </c>
       <c r="F118">
         <v>0.001880877742946708</v>
@@ -4563,10 +4563,10 @@
         <v>247</v>
       </c>
       <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
         <v>1</v>
-      </c>
-      <c r="E119">
-        <v>0</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -4592,10 +4592,10 @@
         <v>248</v>
       </c>
       <c r="D120">
-        <v>0.353053260919173</v>
+        <v>0.003651134133540231</v>
       </c>
       <c r="E120">
-        <v>0.6375336588927936</v>
+        <v>0.9869357856784263</v>
       </c>
       <c r="F120">
         <v>0.009413080188033407</v>
@@ -4621,10 +4621,10 @@
         <v>249</v>
       </c>
       <c r="D121">
-        <v>0.4949308755760369</v>
+        <v>0.003686635944700461</v>
       </c>
       <c r="E121">
-        <v>0.2866359447004608</v>
+        <v>0.7778801843317973</v>
       </c>
       <c r="F121">
         <v>0.2184331797235023</v>
@@ -4650,10 +4650,10 @@
         <v>250</v>
       </c>
       <c r="D122">
-        <v>0.47633959638135</v>
+        <v>0.007654836464857342</v>
       </c>
       <c r="E122">
-        <v>0.477035490605428</v>
+        <v>0.9457202505219207</v>
       </c>
       <c r="F122">
         <v>0.04662491301322199</v>

</xml_diff>